<commit_message>
BFI, MI, 241111 modified 6
</commit_message>
<xml_diff>
--- a/R/data/quiz241104.xlsx
+++ b/R/data/quiz241104.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kwlee/Documents/class202402/R/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A1F22EA-732B-6A40-A02D-546F2AC5F66A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E3EF21E-2B9C-654C-8DE6-0429873F2156}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="48440" yWindow="2580" windowWidth="44800" windowHeight="22940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="47160" yWindow="3860" windowWidth="44800" windowHeight="22940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="설문지 응답 시트1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4546" uniqueCount="947">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5602" uniqueCount="1145">
   <si>
     <t>타임스탬프</t>
   </si>
@@ -2863,6 +2863,600 @@
   </si>
   <si>
     <t>김들</t>
+  </si>
+  <si>
+    <t>leyy2k@naver.com</t>
+  </si>
+  <si>
+    <t>김대현</t>
+  </si>
+  <si>
+    <t>20182346@hallym.ac.kr</t>
+  </si>
+  <si>
+    <t>이용재</t>
+  </si>
+  <si>
+    <t>krdevmon@gmail.com</t>
+  </si>
+  <si>
+    <t>안봉근</t>
+  </si>
+  <si>
+    <t>leedongyoung797@gmail.com</t>
+  </si>
+  <si>
+    <t>이동영</t>
+  </si>
+  <si>
+    <t>njhouuu05@naver.com</t>
+  </si>
+  <si>
+    <t>남진호</t>
+  </si>
+  <si>
+    <t>vcx76613@gmail.com</t>
+  </si>
+  <si>
+    <t>황인태</t>
+  </si>
+  <si>
+    <t>jyl06070@naver.com</t>
+  </si>
+  <si>
+    <t>언론방송융합학과</t>
+  </si>
+  <si>
+    <t>장유림</t>
+  </si>
+  <si>
+    <t>andy041001@naver.com</t>
+  </si>
+  <si>
+    <t>이형범</t>
+  </si>
+  <si>
+    <t>hyerujys2005@naver.com</t>
+  </si>
+  <si>
+    <t>정윤수</t>
+  </si>
+  <si>
+    <t>kms050915@naver.com</t>
+  </si>
+  <si>
+    <t>강명수</t>
+  </si>
+  <si>
+    <t>kmu2916@naver.com</t>
+  </si>
+  <si>
+    <t>강민욱</t>
+  </si>
+  <si>
+    <t>junseok5310@naver.com</t>
+  </si>
+  <si>
+    <t>오준석</t>
+  </si>
+  <si>
+    <t>ssjm9652@naver.com</t>
+  </si>
+  <si>
+    <t>소정민</t>
+  </si>
+  <si>
+    <t>taehwankim05@gmail.com</t>
+  </si>
+  <si>
+    <t>김태환</t>
+  </si>
+  <si>
+    <t>sekhoo313@gmail.com</t>
+  </si>
+  <si>
+    <t>박석호</t>
+  </si>
+  <si>
+    <t>oj5803@naver.com</t>
+  </si>
+  <si>
+    <t>이영주</t>
+  </si>
+  <si>
+    <t>rhoy3156@hallym.ac.kr</t>
+  </si>
+  <si>
+    <t>노원철</t>
+  </si>
+  <si>
+    <t>hg2635394@gmail.com</t>
+  </si>
+  <si>
+    <t>철학과</t>
+  </si>
+  <si>
+    <t>wendy040507@naver.com</t>
+  </si>
+  <si>
+    <t>hanyejun339@gmail.com</t>
+  </si>
+  <si>
+    <t>한예준</t>
+  </si>
+  <si>
+    <t>haeyaxx@naver.com</t>
+  </si>
+  <si>
+    <t>차지혜</t>
+  </si>
+  <si>
+    <t>0524psu@gmail.com</t>
+  </si>
+  <si>
+    <t>박상언</t>
+  </si>
+  <si>
+    <t>you33013301@gmail.com</t>
+  </si>
+  <si>
+    <t>권유정</t>
+  </si>
+  <si>
+    <t>hcheon27@gmail.com</t>
+  </si>
+  <si>
+    <t>천하윤</t>
+  </si>
+  <si>
+    <t>alwo990@naver.com</t>
+  </si>
+  <si>
+    <t>서정웅</t>
+  </si>
+  <si>
+    <t>hsbg1118@gmail.com</t>
+  </si>
+  <si>
+    <t>전희성</t>
+  </si>
+  <si>
+    <t>fred0203@naver.com</t>
+  </si>
+  <si>
+    <t>언어청각학부 청각학전공</t>
+  </si>
+  <si>
+    <t>이강준</t>
+  </si>
+  <si>
+    <t>jyb051128@gmai.com</t>
+  </si>
+  <si>
+    <t>전유빈</t>
+  </si>
+  <si>
+    <t>ghkdxo2003@gmail.com</t>
+  </si>
+  <si>
+    <t>황이준</t>
+  </si>
+  <si>
+    <t>solepkinsg@gmail.com</t>
+  </si>
+  <si>
+    <t>박인성</t>
+  </si>
+  <si>
+    <t>dearmy0819@gmail.com</t>
+  </si>
+  <si>
+    <t>박혜원</t>
+  </si>
+  <si>
+    <t>kby5432@naver.com</t>
+  </si>
+  <si>
+    <t>윤경빈</t>
+  </si>
+  <si>
+    <t>rlaehdnr999@naver.com</t>
+  </si>
+  <si>
+    <t>김도욱</t>
+  </si>
+  <si>
+    <t>chaecjb@naver.com</t>
+  </si>
+  <si>
+    <t>채희수</t>
+  </si>
+  <si>
+    <t>kimteawan347@gmail.com</t>
+  </si>
+  <si>
+    <t>김태완</t>
+  </si>
+  <si>
+    <t>ian5791@naver.com</t>
+  </si>
+  <si>
+    <t>박수현</t>
+  </si>
+  <si>
+    <t>jeongminyoung13@gmail.com</t>
+  </si>
+  <si>
+    <t>정민영</t>
+  </si>
+  <si>
+    <t>a35142191@gmail.com</t>
+  </si>
+  <si>
+    <t>이윤재</t>
+  </si>
+  <si>
+    <t>cmin0945@gmail.com</t>
+  </si>
+  <si>
+    <t>조상민</t>
+  </si>
+  <si>
+    <t>you72460601@gmail.com</t>
+  </si>
+  <si>
+    <t>디지털인문예술</t>
+  </si>
+  <si>
+    <t>유지원</t>
+  </si>
+  <si>
+    <t>yeon4262@naver.com</t>
+  </si>
+  <si>
+    <t>신수연</t>
+  </si>
+  <si>
+    <t>chltjdnjs2421@naver.com</t>
+  </si>
+  <si>
+    <t>최서원</t>
+  </si>
+  <si>
+    <t>aldidhd1112@naver.com</t>
+  </si>
+  <si>
+    <t>권효서</t>
+  </si>
+  <si>
+    <t>mjsong4130@gmail.com</t>
+  </si>
+  <si>
+    <t>송민재</t>
+  </si>
+  <si>
+    <t>soeunjeong0816@naver.com</t>
+  </si>
+  <si>
+    <t>정소은</t>
+  </si>
+  <si>
+    <t>soonbeom1130@naver.com</t>
+  </si>
+  <si>
+    <t>권순범</t>
+  </si>
+  <si>
+    <t>nyo07@naver.com</t>
+  </si>
+  <si>
+    <t>윤효라</t>
+  </si>
+  <si>
+    <t>jb9517asd@naver.com</t>
+  </si>
+  <si>
+    <t>곽우주</t>
+  </si>
+  <si>
+    <t>77sunhwa@gmail.com</t>
+  </si>
+  <si>
+    <t>박선화</t>
+  </si>
+  <si>
+    <t>cgb01045647472@gmail.com</t>
+  </si>
+  <si>
+    <t>경제학고ㅡ</t>
+  </si>
+  <si>
+    <t>최기백</t>
+  </si>
+  <si>
+    <t>sjhaa303028@naver.com</t>
+  </si>
+  <si>
+    <t>신중현</t>
+  </si>
+  <si>
+    <t>his86814189@gmail.com</t>
+  </si>
+  <si>
+    <t>황인성</t>
+  </si>
+  <si>
+    <t>benjamin27@naver.com</t>
+  </si>
+  <si>
+    <t>최재혁</t>
+  </si>
+  <si>
+    <t>ss0001234@naver.com</t>
+  </si>
+  <si>
+    <t>김세은</t>
+  </si>
+  <si>
+    <t>ksong1210@icloud.com</t>
+  </si>
+  <si>
+    <t>곽송</t>
+  </si>
+  <si>
+    <t>huiju4684@naver.com</t>
+  </si>
+  <si>
+    <t>강희주</t>
+  </si>
+  <si>
+    <t>aks186@naver.com</t>
+  </si>
+  <si>
+    <t>안준선</t>
+  </si>
+  <si>
+    <t>seok9431@gmail.com</t>
+  </si>
+  <si>
+    <t>김석주</t>
+  </si>
+  <si>
+    <t>jytoto33@naver.com</t>
+  </si>
+  <si>
+    <t>김지윤</t>
+  </si>
+  <si>
+    <t>Sinyewon921@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">신예원 </t>
+  </si>
+  <si>
+    <t>ade1125@Naver.com</t>
+  </si>
+  <si>
+    <t>안다은</t>
+  </si>
+  <si>
+    <t>yeonju455@naver.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">미래융합스쿨 </t>
+  </si>
+  <si>
+    <t>정연주</t>
+  </si>
+  <si>
+    <t>thddnjs1030@naver.com</t>
+  </si>
+  <si>
+    <t>박송원</t>
+  </si>
+  <si>
+    <t>ydy7495@naver.com</t>
+  </si>
+  <si>
+    <t>윤다연</t>
+  </si>
+  <si>
+    <t>pumio2928@gmail.com</t>
+  </si>
+  <si>
+    <t>bagminhyeog534@gmail.com</t>
+  </si>
+  <si>
+    <t>박민혁</t>
+  </si>
+  <si>
+    <t>nwjcq14@naver.com</t>
+  </si>
+  <si>
+    <t>임미정</t>
+  </si>
+  <si>
+    <t>lgc01040089921@gmail.com</t>
+  </si>
+  <si>
+    <t>이감찬</t>
+  </si>
+  <si>
+    <t>corki1234@naver.com</t>
+  </si>
+  <si>
+    <t>윤서웅</t>
+  </si>
+  <si>
+    <t>7dhw010@gmail.com</t>
+  </si>
+  <si>
+    <t>동형원</t>
+  </si>
+  <si>
+    <t>goeunsue@naver.com</t>
+  </si>
+  <si>
+    <t>고은수</t>
+  </si>
+  <si>
+    <t>fruitekomi@naver.com</t>
+  </si>
+  <si>
+    <t>김예은</t>
+  </si>
+  <si>
+    <t>smsong1036@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">바이오메디컬 </t>
+  </si>
+  <si>
+    <t>송승민</t>
+  </si>
+  <si>
+    <t>dudwndi09@naver.com</t>
+  </si>
+  <si>
+    <t>권영주</t>
+  </si>
+  <si>
+    <t>scjscj913@naver.com</t>
+  </si>
+  <si>
+    <t>최수정</t>
+  </si>
+  <si>
+    <t>juna324a324@naver.com</t>
+  </si>
+  <si>
+    <t>정준우</t>
+  </si>
+  <si>
+    <t>tlsh1282@naver.com</t>
+  </si>
+  <si>
+    <t>원세한</t>
+  </si>
+  <si>
+    <t>leeleeya1013@gmail.com</t>
+  </si>
+  <si>
+    <t>김민서</t>
+  </si>
+  <si>
+    <t>sowon051125@naver.com</t>
+  </si>
+  <si>
+    <t>이소원</t>
+  </si>
+  <si>
+    <t>jeongeun20050618@gmail.com</t>
+  </si>
+  <si>
+    <t>권정은</t>
+  </si>
+  <si>
+    <t>tmddl3538@naver.com</t>
+  </si>
+  <si>
+    <t>이승재</t>
+  </si>
+  <si>
+    <t>pjy35870859@gmail.com</t>
+  </si>
+  <si>
+    <t>박지연</t>
+  </si>
+  <si>
+    <t>hmg4898@naver.com</t>
+  </si>
+  <si>
+    <t>한민교</t>
+  </si>
+  <si>
+    <t>bhyejin420@gmail.com</t>
+  </si>
+  <si>
+    <t>박혜진</t>
+  </si>
+  <si>
+    <t>dlalstmd03@gmail.com</t>
+  </si>
+  <si>
+    <t>이민승</t>
+  </si>
+  <si>
+    <t>abc6518@gmail.com</t>
+  </si>
+  <si>
+    <t>반도체</t>
+  </si>
+  <si>
+    <t>박상준</t>
+  </si>
+  <si>
+    <t>tjtkdwns0909@naver.com</t>
+  </si>
+  <si>
+    <t>서상준</t>
+  </si>
+  <si>
+    <t>bamddol2@gmail.com</t>
+  </si>
+  <si>
+    <t>조찬영</t>
+  </si>
+  <si>
+    <t>yeona0926@gmail.com</t>
+  </si>
+  <si>
+    <t>강연아</t>
+  </si>
+  <si>
+    <t>kdhmonkeyking@gmail.com</t>
+  </si>
+  <si>
+    <t>김동현</t>
+  </si>
+  <si>
+    <t>solar08230@naver.com</t>
+  </si>
+  <si>
+    <t>안다빈</t>
+  </si>
+  <si>
+    <t>tlsdmsco1130@naver.com</t>
+  </si>
+  <si>
+    <t>신은채</t>
+  </si>
+  <si>
+    <t>skaskgus@gmail.com</t>
+  </si>
+  <si>
+    <t>남나현</t>
+  </si>
+  <si>
+    <t>xodet0817@naver.com</t>
+  </si>
+  <si>
+    <t>문종윤</t>
+  </si>
+  <si>
+    <t>hizero0223@naver.com</t>
+  </si>
+  <si>
+    <t>조하영</t>
+  </si>
+  <si>
+    <t>jangjunhyeok1001@naver.com</t>
+  </si>
+  <si>
+    <t>빈도체 디스플레이</t>
+  </si>
+  <si>
+    <t>장준혁</t>
   </si>
 </sst>
 </file>
@@ -3273,7 +3867,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Form_Responses1" displayName="Form_Responses1" ref="A1:N413" headerRowCount="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Form_Responses1" displayName="Form_Responses1" ref="A1:N509" headerRowCount="0">
   <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Column1"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Column2"/>
@@ -3500,11 +4094,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:N413"/>
+  <dimension ref="A1:N509"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A368" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A420" sqref="A420"/>
+      <pane ySplit="1" topLeftCell="A471" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C520" sqref="C520"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -20453,10 +21047,3946 @@
       <c r="L413" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="M413" s="20"/>
       <c r="N413" s="19" t="s">
         <v>33</v>
       </c>
+    </row>
+    <row r="414" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A414" s="4">
+        <v>45611.730239895835</v>
+      </c>
+      <c r="B414" s="5" t="s">
+        <v>947</v>
+      </c>
+      <c r="C414" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="D414" s="5">
+        <v>20215115</v>
+      </c>
+      <c r="E414" s="5" t="s">
+        <v>948</v>
+      </c>
+      <c r="F414" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G414" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H414" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I414" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J414" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="K414" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="L414" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="M414" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="415" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A415" s="7">
+        <v>45611.882505775458</v>
+      </c>
+      <c r="B415" s="8" t="s">
+        <v>949</v>
+      </c>
+      <c r="C415" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="D415" s="8">
+        <v>20182346</v>
+      </c>
+      <c r="E415" s="8" t="s">
+        <v>950</v>
+      </c>
+      <c r="F415" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G415" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="H415" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I415" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J415" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="K415" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="L415" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="M415" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="416" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A416" s="4">
+        <v>45611.932433275462</v>
+      </c>
+      <c r="B416" s="5" t="s">
+        <v>951</v>
+      </c>
+      <c r="C416" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="D416" s="5">
+        <v>20205198</v>
+      </c>
+      <c r="E416" s="5" t="s">
+        <v>952</v>
+      </c>
+      <c r="F416" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G416" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H416" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="I416" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J416" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="K416" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="L416" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N416" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="417" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A417" s="7">
+        <v>45611.946005289356</v>
+      </c>
+      <c r="B417" s="8" t="s">
+        <v>953</v>
+      </c>
+      <c r="C417" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D417" s="8">
+        <v>20243934</v>
+      </c>
+      <c r="E417" s="8" t="s">
+        <v>954</v>
+      </c>
+      <c r="F417" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G417" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H417" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="I417" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J417" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K417" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="L417" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="M417" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="418" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A418" s="4">
+        <v>45611.949060694446</v>
+      </c>
+      <c r="B418" s="5" t="s">
+        <v>955</v>
+      </c>
+      <c r="C418" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="D418" s="5">
+        <v>20245156</v>
+      </c>
+      <c r="E418" s="5" t="s">
+        <v>956</v>
+      </c>
+      <c r="F418" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G418" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H418" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="I418" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J418" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="K418" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="L418" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="M418" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="419" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A419" s="7">
+        <v>45611.962285879628</v>
+      </c>
+      <c r="B419" s="8" t="s">
+        <v>957</v>
+      </c>
+      <c r="C419" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="D419" s="8">
+        <v>20246306</v>
+      </c>
+      <c r="E419" s="8" t="s">
+        <v>958</v>
+      </c>
+      <c r="F419" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G419" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="H419" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I419" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="J419" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K419" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="L419" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="N419" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="420" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A420" s="4">
+        <v>45611.968249803242</v>
+      </c>
+      <c r="B420" s="5" t="s">
+        <v>959</v>
+      </c>
+      <c r="C420" s="5" t="s">
+        <v>960</v>
+      </c>
+      <c r="D420" s="5">
+        <v>20212749</v>
+      </c>
+      <c r="E420" s="5" t="s">
+        <v>961</v>
+      </c>
+      <c r="F420" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="G420" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="H420" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="I420" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J420" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="K420" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="L420" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N420" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="421" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A421" s="7">
+        <v>45611.979570023148</v>
+      </c>
+      <c r="B421" s="8" t="s">
+        <v>962</v>
+      </c>
+      <c r="C421" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="D421" s="8">
+        <v>20231720</v>
+      </c>
+      <c r="E421" s="8" t="s">
+        <v>963</v>
+      </c>
+      <c r="F421" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G421" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H421" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="I421" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J421" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="K421" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="L421" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="N421" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="422" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A422" s="4">
+        <v>45612.009399756949</v>
+      </c>
+      <c r="B422" s="5" t="s">
+        <v>964</v>
+      </c>
+      <c r="C422" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D422" s="5">
+        <v>20242575</v>
+      </c>
+      <c r="E422" s="5" t="s">
+        <v>965</v>
+      </c>
+      <c r="F422" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="G422" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H422" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I422" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J422" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="K422" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="L422" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="M422" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="423" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A423" s="7">
+        <v>45612.068824502319</v>
+      </c>
+      <c r="B423" s="8" t="s">
+        <v>966</v>
+      </c>
+      <c r="C423" s="8" t="s">
+        <v>475</v>
+      </c>
+      <c r="D423" s="8">
+        <v>20246902</v>
+      </c>
+      <c r="E423" s="8" t="s">
+        <v>967</v>
+      </c>
+      <c r="F423" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G423" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H423" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="I423" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J423" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K423" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="L423" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="N423" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="424" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A424" s="4">
+        <v>45612.100836423611</v>
+      </c>
+      <c r="B424" s="5" t="s">
+        <v>968</v>
+      </c>
+      <c r="C424" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D424" s="5">
+        <v>20222902</v>
+      </c>
+      <c r="E424" s="5" t="s">
+        <v>969</v>
+      </c>
+      <c r="F424" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G424" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H424" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I424" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J424" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="K424" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="L424" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N424" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="425" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A425" s="7">
+        <v>45612.114189247688</v>
+      </c>
+      <c r="B425" s="8" t="s">
+        <v>970</v>
+      </c>
+      <c r="C425" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="D425" s="8">
+        <v>20193626</v>
+      </c>
+      <c r="E425" s="8" t="s">
+        <v>971</v>
+      </c>
+      <c r="F425" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G425" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="H425" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="I425" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J425" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="K425" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="L425" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="N425" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="426" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A426" s="4">
+        <v>45612.117302048609</v>
+      </c>
+      <c r="B426" s="5" t="s">
+        <v>972</v>
+      </c>
+      <c r="C426" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D426" s="5">
+        <v>20241047</v>
+      </c>
+      <c r="E426" s="5" t="s">
+        <v>973</v>
+      </c>
+      <c r="F426" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G426" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H426" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I426" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J426" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="K426" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="L426" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N426" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="427" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A427" s="7">
+        <v>45612.131687187502</v>
+      </c>
+      <c r="B427" s="8" t="s">
+        <v>974</v>
+      </c>
+      <c r="C427" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="D427" s="8">
+        <v>20242411</v>
+      </c>
+      <c r="E427" s="8" t="s">
+        <v>975</v>
+      </c>
+      <c r="F427" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G427" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H427" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="I427" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="J427" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="K427" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="L427" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="N427" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="428" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A428" s="4">
+        <v>45612.219688043981</v>
+      </c>
+      <c r="B428" s="5" t="s">
+        <v>976</v>
+      </c>
+      <c r="C428" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D428" s="5">
+        <v>20241038</v>
+      </c>
+      <c r="E428" s="5" t="s">
+        <v>977</v>
+      </c>
+      <c r="F428" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G428" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H428" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I428" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="J428" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="K428" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="L428" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="M428" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="429" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A429" s="7">
+        <v>45612.331247094902</v>
+      </c>
+      <c r="B429" s="8" t="s">
+        <v>978</v>
+      </c>
+      <c r="C429" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D429" s="8">
+        <v>20242628</v>
+      </c>
+      <c r="E429" s="8" t="s">
+        <v>979</v>
+      </c>
+      <c r="F429" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G429" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H429" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="I429" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J429" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="K429" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="L429" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="N429" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="430" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A430" s="4">
+        <v>45612.375846967596</v>
+      </c>
+      <c r="B430" s="5" t="s">
+        <v>980</v>
+      </c>
+      <c r="C430" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="D430" s="5">
+        <v>20202719</v>
+      </c>
+      <c r="E430" s="5" t="s">
+        <v>981</v>
+      </c>
+      <c r="F430" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G430" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H430" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="I430" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J430" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="K430" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="L430" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="M430" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="431" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A431" s="17">
+        <v>45612.432631874995</v>
+      </c>
+      <c r="B431" s="18" t="s">
+        <v>982</v>
+      </c>
+      <c r="C431" s="18" t="s">
+        <v>983</v>
+      </c>
+      <c r="D431" s="18">
+        <v>20231033</v>
+      </c>
+      <c r="E431" s="18" t="s">
+        <v>936</v>
+      </c>
+      <c r="F431" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="G431" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="H431" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="I431" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="J431" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="K431" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="L431" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="M431" s="18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="432" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A432" s="4">
+        <v>45612.470198055555</v>
+      </c>
+      <c r="B432" s="5" t="s">
+        <v>984</v>
+      </c>
+      <c r="C432" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D432" s="5">
+        <v>20243002</v>
+      </c>
+      <c r="E432" s="5" t="s">
+        <v>911</v>
+      </c>
+      <c r="F432" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G432" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H432" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="I432" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J432" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="K432" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="L432" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="M432" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="433" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A433" s="7">
+        <v>45612.485488738428</v>
+      </c>
+      <c r="B433" s="8" t="s">
+        <v>985</v>
+      </c>
+      <c r="C433" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="D433" s="8">
+        <v>20246649</v>
+      </c>
+      <c r="E433" s="8" t="s">
+        <v>986</v>
+      </c>
+      <c r="F433" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G433" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H433" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I433" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="J433" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="K433" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="L433" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="N433" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="434" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A434" s="4">
+        <v>45612.558727638891</v>
+      </c>
+      <c r="B434" s="5" t="s">
+        <v>987</v>
+      </c>
+      <c r="C434" s="5" t="s">
+        <v>750</v>
+      </c>
+      <c r="D434" s="5">
+        <v>20212846</v>
+      </c>
+      <c r="E434" s="5" t="s">
+        <v>988</v>
+      </c>
+      <c r="F434" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G434" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H434" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I434" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J434" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="K434" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="L434" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N434" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="435" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A435" s="7">
+        <v>45612.563427349538</v>
+      </c>
+      <c r="B435" s="8" t="s">
+        <v>989</v>
+      </c>
+      <c r="C435" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D435" s="8">
+        <v>20243712</v>
+      </c>
+      <c r="E435" s="8" t="s">
+        <v>990</v>
+      </c>
+      <c r="F435" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G435" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="H435" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="I435" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J435" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="K435" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="L435" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="M435" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="436" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A436" s="4">
+        <v>45612.571233391209</v>
+      </c>
+      <c r="B436" s="5" t="s">
+        <v>991</v>
+      </c>
+      <c r="C436" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="D436" s="5">
+        <v>20223504</v>
+      </c>
+      <c r="E436" s="5" t="s">
+        <v>992</v>
+      </c>
+      <c r="F436" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G436" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H436" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="I436" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J436" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="K436" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="L436" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N436" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="437" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A437" s="7">
+        <v>45612.584156053243</v>
+      </c>
+      <c r="B437" s="8" t="s">
+        <v>993</v>
+      </c>
+      <c r="C437" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="D437" s="8">
+        <v>20246293</v>
+      </c>
+      <c r="E437" s="8" t="s">
+        <v>994</v>
+      </c>
+      <c r="F437" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G437" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="H437" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I437" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J437" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="K437" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="L437" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="N437" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="438" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A438" s="4">
+        <v>45612.61387361111</v>
+      </c>
+      <c r="B438" s="5" t="s">
+        <v>995</v>
+      </c>
+      <c r="C438" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="D438" s="5">
+        <v>20207133</v>
+      </c>
+      <c r="E438" s="5" t="s">
+        <v>996</v>
+      </c>
+      <c r="F438" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G438" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="H438" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="I438" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J438" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="K438" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="L438" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="M438" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="439" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A439" s="7">
+        <v>45612.626374363426</v>
+      </c>
+      <c r="B439" s="8" t="s">
+        <v>997</v>
+      </c>
+      <c r="C439" s="8" t="s">
+        <v>328</v>
+      </c>
+      <c r="D439" s="8">
+        <v>20246770</v>
+      </c>
+      <c r="E439" s="8" t="s">
+        <v>998</v>
+      </c>
+      <c r="F439" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G439" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H439" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="I439" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J439" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="K439" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="L439" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="M439" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="440" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A440" s="4">
+        <v>45612.635355706021</v>
+      </c>
+      <c r="B440" s="5" t="s">
+        <v>999</v>
+      </c>
+      <c r="C440" s="5" t="s">
+        <v>1000</v>
+      </c>
+      <c r="D440" s="5">
+        <v>20227091</v>
+      </c>
+      <c r="E440" s="5" t="s">
+        <v>1001</v>
+      </c>
+      <c r="F440" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G440" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H440" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="I440" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J440" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="K440" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="L440" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="M440" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="441" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A441" s="7">
+        <v>45612.63832795139</v>
+      </c>
+      <c r="B441" s="8" t="s">
+        <v>1002</v>
+      </c>
+      <c r="C441" s="8" t="s">
+        <v>609</v>
+      </c>
+      <c r="D441" s="8">
+        <v>20243646</v>
+      </c>
+      <c r="E441" s="8" t="s">
+        <v>1003</v>
+      </c>
+      <c r="F441" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G441" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="H441" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="I441" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J441" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="K441" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="L441" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="N441" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="442" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A442" s="4">
+        <v>45612.652372268523</v>
+      </c>
+      <c r="B442" s="5" t="s">
+        <v>1004</v>
+      </c>
+      <c r="C442" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="D442" s="5">
+        <v>20231733</v>
+      </c>
+      <c r="E442" s="5" t="s">
+        <v>1005</v>
+      </c>
+      <c r="F442" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G442" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H442" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I442" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J442" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="K442" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="L442" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N442" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="443" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A443" s="7">
+        <v>45612.666778449071</v>
+      </c>
+      <c r="B443" s="8" t="s">
+        <v>1006</v>
+      </c>
+      <c r="C443" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D443" s="8">
+        <v>20236615</v>
+      </c>
+      <c r="E443" s="8" t="s">
+        <v>1007</v>
+      </c>
+      <c r="F443" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G443" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="H443" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="I443" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J443" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="K443" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="L443" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="M443" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="444" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A444" s="13">
+        <v>45612.673797627314</v>
+      </c>
+      <c r="B444" s="14" t="s">
+        <v>1008</v>
+      </c>
+      <c r="C444" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="D444" s="14">
+        <v>20243225</v>
+      </c>
+      <c r="E444" s="14" t="s">
+        <v>1009</v>
+      </c>
+      <c r="F444" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="G444" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="H444" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="I444" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="J444" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="K444" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="L444" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="N444" s="15" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="445" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A445" s="7">
+        <v>45612.705149722227</v>
+      </c>
+      <c r="B445" s="8" t="s">
+        <v>1010</v>
+      </c>
+      <c r="C445" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="D445" s="8">
+        <v>20192737</v>
+      </c>
+      <c r="E445" s="8" t="s">
+        <v>1011</v>
+      </c>
+      <c r="F445" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G445" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H445" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="I445" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="J445" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="K445" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="L445" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="M445" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="446" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A446" s="4">
+        <v>45612.718481944445</v>
+      </c>
+      <c r="B446" s="5" t="s">
+        <v>1012</v>
+      </c>
+      <c r="C446" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D446" s="5">
+        <v>20221007</v>
+      </c>
+      <c r="E446" s="5" t="s">
+        <v>1013</v>
+      </c>
+      <c r="F446" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G446" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H446" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I446" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J446" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="K446" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="L446" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N446" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="447" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A447" s="7">
+        <v>45612.725065937499</v>
+      </c>
+      <c r="B447" s="8" t="s">
+        <v>1014</v>
+      </c>
+      <c r="C447" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D447" s="8">
+        <v>20203046</v>
+      </c>
+      <c r="E447" s="8" t="s">
+        <v>1015</v>
+      </c>
+      <c r="F447" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G447" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="H447" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="I447" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J447" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="K447" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="L447" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="M447" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="448" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A448" s="4">
+        <v>45612.735888298615</v>
+      </c>
+      <c r="B448" s="5" t="s">
+        <v>1016</v>
+      </c>
+      <c r="C448" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D448" s="5">
+        <v>20212613</v>
+      </c>
+      <c r="E448" s="5" t="s">
+        <v>1017</v>
+      </c>
+      <c r="F448" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G448" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H448" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="I448" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J448" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="K448" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="L448" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="M448" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="449" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A449" s="7">
+        <v>45612.738068946761</v>
+      </c>
+      <c r="B449" s="8" t="s">
+        <v>1018</v>
+      </c>
+      <c r="C449" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="D449" s="8">
+        <v>20241520</v>
+      </c>
+      <c r="E449" s="8" t="s">
+        <v>1019</v>
+      </c>
+      <c r="F449" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G449" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="H449" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="I449" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J449" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="K449" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="L449" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="N449" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="450" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A450" s="4">
+        <v>45612.76220438657</v>
+      </c>
+      <c r="B450" s="5" t="s">
+        <v>1020</v>
+      </c>
+      <c r="C450" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D450" s="5">
+        <v>20246281</v>
+      </c>
+      <c r="E450" s="5" t="s">
+        <v>1021</v>
+      </c>
+      <c r="F450" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G450" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H450" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I450" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J450" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="K450" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="L450" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="M450" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="451" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A451" s="7">
+        <v>45612.764578425922</v>
+      </c>
+      <c r="B451" s="8" t="s">
+        <v>1022</v>
+      </c>
+      <c r="C451" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="D451" s="8">
+        <v>20243241</v>
+      </c>
+      <c r="E451" s="8" t="s">
+        <v>1023</v>
+      </c>
+      <c r="F451" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G451" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="H451" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="I451" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J451" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="K451" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="L451" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="N451" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="452" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A452" s="4">
+        <v>45612.784676655094</v>
+      </c>
+      <c r="B452" s="5" t="s">
+        <v>1024</v>
+      </c>
+      <c r="C452" s="5" t="s">
+        <v>328</v>
+      </c>
+      <c r="D452" s="5">
+        <v>20246776</v>
+      </c>
+      <c r="E452" s="5" t="s">
+        <v>1025</v>
+      </c>
+      <c r="F452" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G452" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H452" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="I452" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J452" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="K452" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="L452" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="M452" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="453" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A453" s="7">
+        <v>45612.786899120372</v>
+      </c>
+      <c r="B453" s="8" t="s">
+        <v>1026</v>
+      </c>
+      <c r="C453" s="8" t="s">
+        <v>1027</v>
+      </c>
+      <c r="D453" s="8">
+        <v>20201721</v>
+      </c>
+      <c r="E453" s="8" t="s">
+        <v>1028</v>
+      </c>
+      <c r="F453" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G453" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="H453" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="I453" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J453" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="K453" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="L453" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="M453" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="454" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A454" s="4">
+        <v>45612.808671956023</v>
+      </c>
+      <c r="B454" s="5" t="s">
+        <v>1029</v>
+      </c>
+      <c r="C454" s="5" t="s">
+        <v>536</v>
+      </c>
+      <c r="D454" s="5">
+        <v>20223325</v>
+      </c>
+      <c r="E454" s="5" t="s">
+        <v>1030</v>
+      </c>
+      <c r="F454" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G454" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H454" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I454" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J454" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="K454" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="L454" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N454" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="455" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A455" s="7">
+        <v>45612.822202615745</v>
+      </c>
+      <c r="B455" s="8" t="s">
+        <v>1031</v>
+      </c>
+      <c r="C455" s="8" t="s">
+        <v>292</v>
+      </c>
+      <c r="D455" s="8">
+        <v>20242848</v>
+      </c>
+      <c r="E455" s="8" t="s">
+        <v>1032</v>
+      </c>
+      <c r="F455" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G455" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="H455" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I455" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J455" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="K455" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="L455" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="N455" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="456" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A456" s="4">
+        <v>45612.860398032411</v>
+      </c>
+      <c r="B456" s="5" t="s">
+        <v>1033</v>
+      </c>
+      <c r="C456" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D456" s="5">
+        <v>20172808</v>
+      </c>
+      <c r="E456" s="5" t="s">
+        <v>1034</v>
+      </c>
+      <c r="F456" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G456" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H456" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="I456" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J456" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="K456" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="L456" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N456" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="457" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A457" s="7">
+        <v>45612.865795659724</v>
+      </c>
+      <c r="B457" s="8" t="s">
+        <v>1035</v>
+      </c>
+      <c r="C457" s="8" t="s">
+        <v>328</v>
+      </c>
+      <c r="D457" s="8">
+        <v>20236736</v>
+      </c>
+      <c r="E457" s="8" t="s">
+        <v>1036</v>
+      </c>
+      <c r="F457" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G457" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="H457" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="I457" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J457" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="K457" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="L457" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="N457" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="458" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A458" s="4">
+        <v>45612.866383159722</v>
+      </c>
+      <c r="B458" s="5" t="s">
+        <v>1037</v>
+      </c>
+      <c r="C458" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="D458" s="5">
+        <v>20243648</v>
+      </c>
+      <c r="E458" s="5" t="s">
+        <v>1038</v>
+      </c>
+      <c r="F458" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G458" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H458" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I458" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J458" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="K458" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="L458" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N458" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="459" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A459" s="17">
+        <v>45612.874275092589</v>
+      </c>
+      <c r="B459" s="18" t="s">
+        <v>1039</v>
+      </c>
+      <c r="C459" s="18" t="s">
+        <v>437</v>
+      </c>
+      <c r="D459" s="18">
+        <v>20235112</v>
+      </c>
+      <c r="E459" s="18" t="s">
+        <v>1040</v>
+      </c>
+      <c r="F459" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="G459" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="H459" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="I459" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="J459" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="K459" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="L459" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="N459" s="19" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="460" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A460" s="4">
+        <v>45612.928333414355</v>
+      </c>
+      <c r="B460" s="5" t="s">
+        <v>1041</v>
+      </c>
+      <c r="C460" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D460" s="5">
+        <v>20217087</v>
+      </c>
+      <c r="E460" s="5" t="s">
+        <v>1042</v>
+      </c>
+      <c r="F460" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G460" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H460" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="I460" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J460" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="K460" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="L460" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="M460" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="461" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A461" s="7">
+        <v>45612.929197025464</v>
+      </c>
+      <c r="B461" s="8" t="s">
+        <v>1043</v>
+      </c>
+      <c r="C461" s="8" t="s">
+        <v>277</v>
+      </c>
+      <c r="D461" s="8">
+        <v>20245109</v>
+      </c>
+      <c r="E461" s="8" t="s">
+        <v>1044</v>
+      </c>
+      <c r="F461" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G461" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H461" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="I461" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J461" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="K461" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="L461" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="M461" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="462" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A462" s="4">
+        <v>45612.948725046299</v>
+      </c>
+      <c r="B462" s="5" t="s">
+        <v>1045</v>
+      </c>
+      <c r="C462" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D462" s="5">
+        <v>20242956</v>
+      </c>
+      <c r="E462" s="5" t="s">
+        <v>1046</v>
+      </c>
+      <c r="F462" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G462" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H462" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I462" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J462" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="K462" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="L462" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="M462" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="463" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A463" s="7">
+        <v>45612.949796701389</v>
+      </c>
+      <c r="B463" s="8" t="s">
+        <v>1047</v>
+      </c>
+      <c r="C463" s="8" t="s">
+        <v>1048</v>
+      </c>
+      <c r="D463" s="8">
+        <v>20193003</v>
+      </c>
+      <c r="E463" s="8" t="s">
+        <v>1049</v>
+      </c>
+      <c r="F463" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G463" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H463" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="I463" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J463" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="K463" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="L463" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="N463" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="464" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A464" s="4">
+        <v>45612.949883356487</v>
+      </c>
+      <c r="B464" s="5" t="s">
+        <v>1050</v>
+      </c>
+      <c r="C464" s="5" t="s">
+        <v>328</v>
+      </c>
+      <c r="D464" s="5">
+        <v>20246741</v>
+      </c>
+      <c r="E464" s="5" t="s">
+        <v>1051</v>
+      </c>
+      <c r="F464" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G464" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H464" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="I464" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J464" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="K464" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="L464" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N464" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="465" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A465" s="7">
+        <v>45612.950887754632</v>
+      </c>
+      <c r="B465" s="8" t="s">
+        <v>1052</v>
+      </c>
+      <c r="C465" s="8" t="s">
+        <v>475</v>
+      </c>
+      <c r="D465" s="8">
+        <v>20246942</v>
+      </c>
+      <c r="E465" s="8" t="s">
+        <v>1053</v>
+      </c>
+      <c r="F465" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G465" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="H465" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="I465" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J465" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="K465" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="L465" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="M465" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="466" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A466" s="4">
+        <v>45612.953949363422</v>
+      </c>
+      <c r="B466" s="5" t="s">
+        <v>1054</v>
+      </c>
+      <c r="C466" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="D466" s="5">
+        <v>20212583</v>
+      </c>
+      <c r="E466" s="5" t="s">
+        <v>1055</v>
+      </c>
+      <c r="F466" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G466" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H466" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I466" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J466" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="K466" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="L466" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="M466" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="467" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A467" s="7">
+        <v>45612.954838877311</v>
+      </c>
+      <c r="B467" s="8" t="s">
+        <v>1056</v>
+      </c>
+      <c r="C467" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D467" s="8">
+        <v>20203211</v>
+      </c>
+      <c r="E467" s="8" t="s">
+        <v>1057</v>
+      </c>
+      <c r="F467" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G467" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="H467" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I467" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J467" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="K467" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="L467" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="M467" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="468" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A468" s="4">
+        <v>45612.959829861109</v>
+      </c>
+      <c r="B468" s="5" t="s">
+        <v>1058</v>
+      </c>
+      <c r="C468" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="D468" s="5">
+        <v>20242304</v>
+      </c>
+      <c r="E468" s="5" t="s">
+        <v>1059</v>
+      </c>
+      <c r="F468" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G468" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H468" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="I468" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J468" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="K468" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="L468" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="M468" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="469" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A469" s="7">
+        <v>45612.962357071759</v>
+      </c>
+      <c r="B469" s="8" t="s">
+        <v>1060</v>
+      </c>
+      <c r="C469" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D469" s="8">
+        <v>20217097</v>
+      </c>
+      <c r="E469" s="8" t="s">
+        <v>1061</v>
+      </c>
+      <c r="F469" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G469" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="H469" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="I469" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="J469" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="K469" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="L469" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="N469" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="470" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A470" s="4">
+        <v>45612.963402280089</v>
+      </c>
+      <c r="B470" s="5" t="s">
+        <v>1062</v>
+      </c>
+      <c r="C470" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="D470" s="5">
+        <v>20232728</v>
+      </c>
+      <c r="E470" s="5" t="s">
+        <v>1063</v>
+      </c>
+      <c r="F470" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G470" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H470" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I470" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J470" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="K470" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="L470" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N470" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="471" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A471" s="7">
+        <v>45612.964917928242</v>
+      </c>
+      <c r="B471" s="8" t="s">
+        <v>1064</v>
+      </c>
+      <c r="C471" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D471" s="8">
+        <v>20243907</v>
+      </c>
+      <c r="E471" s="8" t="s">
+        <v>1065</v>
+      </c>
+      <c r="F471" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="G471" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="H471" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I471" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="J471" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="K471" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="L471" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="M471" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="472" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A472" s="4">
+        <v>45612.965812430557</v>
+      </c>
+      <c r="B472" s="5" t="s">
+        <v>1066</v>
+      </c>
+      <c r="C472" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D472" s="5">
+        <v>20243912</v>
+      </c>
+      <c r="E472" s="5" t="s">
+        <v>1067</v>
+      </c>
+      <c r="F472" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G472" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H472" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="I472" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J472" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="K472" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="L472" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="M472" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="473" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A473" s="7">
+        <v>45612.970257546302</v>
+      </c>
+      <c r="B473" s="8" t="s">
+        <v>1068</v>
+      </c>
+      <c r="C473" s="8" t="s">
+        <v>694</v>
+      </c>
+      <c r="D473" s="8">
+        <v>20243821</v>
+      </c>
+      <c r="E473" s="8" t="s">
+        <v>1069</v>
+      </c>
+      <c r="F473" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G473" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="H473" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="I473" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J473" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K473" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="L473" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="M473" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="474" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A474" s="4">
+        <v>45612.974622534719</v>
+      </c>
+      <c r="B474" s="5" t="s">
+        <v>1070</v>
+      </c>
+      <c r="C474" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D474" s="5">
+        <v>20232548</v>
+      </c>
+      <c r="E474" s="5" t="s">
+        <v>1071</v>
+      </c>
+      <c r="F474" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G474" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H474" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="I474" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J474" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="K474" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="L474" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N474" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="475" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A475" s="7">
+        <v>45612.983189085644</v>
+      </c>
+      <c r="B475" s="8" t="s">
+        <v>1072</v>
+      </c>
+      <c r="C475" s="8" t="s">
+        <v>1073</v>
+      </c>
+      <c r="D475" s="8">
+        <v>20226638</v>
+      </c>
+      <c r="E475" s="8" t="s">
+        <v>1074</v>
+      </c>
+      <c r="F475" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G475" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="H475" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="I475" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J475" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="K475" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="L475" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="N475" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="476" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A476" s="4">
+        <v>45612.988480879634</v>
+      </c>
+      <c r="B476" s="5" t="s">
+        <v>1075</v>
+      </c>
+      <c r="C476" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="D476" s="5">
+        <v>20171035</v>
+      </c>
+      <c r="E476" s="5" t="s">
+        <v>1076</v>
+      </c>
+      <c r="F476" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="G476" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H476" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I476" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J476" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="K476" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="L476" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="M476" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="477" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A477" s="7">
+        <v>45612.988603657403</v>
+      </c>
+      <c r="B477" s="8" t="s">
+        <v>1077</v>
+      </c>
+      <c r="C477" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="D477" s="8">
+        <v>20242423</v>
+      </c>
+      <c r="E477" s="8" t="s">
+        <v>1078</v>
+      </c>
+      <c r="F477" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G477" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="H477" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="I477" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J477" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="K477" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="L477" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="N477" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="478" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A478" s="13">
+        <v>45612.993292395833</v>
+      </c>
+      <c r="B478" s="14" t="s">
+        <v>1079</v>
+      </c>
+      <c r="C478" s="14" t="s">
+        <v>829</v>
+      </c>
+      <c r="D478" s="14">
+        <v>20232527</v>
+      </c>
+      <c r="E478" s="14" t="s">
+        <v>347</v>
+      </c>
+      <c r="F478" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="G478" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="H478" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="I478" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="J478" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="K478" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="L478" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="N478" s="15" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="479" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A479" s="7">
+        <v>45612.995437627316</v>
+      </c>
+      <c r="B479" s="8" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C479" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="D479" s="8">
+        <v>20242320</v>
+      </c>
+      <c r="E479" s="8" t="s">
+        <v>1081</v>
+      </c>
+      <c r="F479" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G479" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H479" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="I479" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J479" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K479" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="L479" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="N479" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="480" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A480" s="4">
+        <v>45612.996029560185</v>
+      </c>
+      <c r="B480" s="5" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C480" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="D480" s="5">
+        <v>20216631</v>
+      </c>
+      <c r="E480" s="5" t="s">
+        <v>1083</v>
+      </c>
+      <c r="F480" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G480" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H480" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="I480" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="J480" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="K480" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="L480" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="M480" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="481" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A481" s="7">
+        <v>45612.999638773152</v>
+      </c>
+      <c r="B481" s="8" t="s">
+        <v>1084</v>
+      </c>
+      <c r="C481" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D481" s="8">
+        <v>20242995</v>
+      </c>
+      <c r="E481" s="8" t="s">
+        <v>1085</v>
+      </c>
+      <c r="F481" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G481" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="H481" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="I481" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J481" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K481" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="L481" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="M481" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="482" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A482" s="4">
+        <v>45613.011663206024</v>
+      </c>
+      <c r="B482" s="5" t="s">
+        <v>1086</v>
+      </c>
+      <c r="C482" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="D482" s="5">
+        <v>20211523</v>
+      </c>
+      <c r="E482" s="5" t="s">
+        <v>1087</v>
+      </c>
+      <c r="F482" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G482" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H482" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I482" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="J482" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="K482" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="L482" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="M482" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="483" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A483" s="7">
+        <v>45613.013127256942</v>
+      </c>
+      <c r="B483" s="8" t="s">
+        <v>1088</v>
+      </c>
+      <c r="C483" s="8" t="s">
+        <v>536</v>
+      </c>
+      <c r="D483" s="8">
+        <v>20243314</v>
+      </c>
+      <c r="E483" s="8" t="s">
+        <v>1089</v>
+      </c>
+      <c r="F483" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G483" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H483" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="I483" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J483" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K483" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="L483" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="M483" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="484" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A484" s="4">
+        <v>45613.015794930558</v>
+      </c>
+      <c r="B484" s="5" t="s">
+        <v>1090</v>
+      </c>
+      <c r="C484" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D484" s="5">
+        <v>20242907</v>
+      </c>
+      <c r="E484" s="5" t="s">
+        <v>1091</v>
+      </c>
+      <c r="F484" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G484" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H484" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="I484" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J484" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="K484" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="L484" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N484" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="485" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A485" s="7">
+        <v>45613.022533217591</v>
+      </c>
+      <c r="B485" s="8" t="s">
+        <v>1092</v>
+      </c>
+      <c r="C485" s="8" t="s">
+        <v>609</v>
+      </c>
+      <c r="D485" s="8">
+        <v>20233710</v>
+      </c>
+      <c r="E485" s="8" t="s">
+        <v>1093</v>
+      </c>
+      <c r="F485" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G485" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="H485" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="I485" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J485" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="K485" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="L485" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="N485" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="486" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A486" s="4">
+        <v>45613.023515844907</v>
+      </c>
+      <c r="B486" s="5" t="s">
+        <v>1094</v>
+      </c>
+      <c r="C486" s="5" t="s">
+        <v>1095</v>
+      </c>
+      <c r="D486" s="5">
+        <v>20243624</v>
+      </c>
+      <c r="E486" s="5" t="s">
+        <v>1096</v>
+      </c>
+      <c r="F486" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G486" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="H486" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I486" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J486" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="K486" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="L486" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="M486" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="487" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A487" s="7">
+        <v>45613.02973790509</v>
+      </c>
+      <c r="B487" s="8" t="s">
+        <v>1097</v>
+      </c>
+      <c r="C487" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D487" s="8">
+        <v>20212603</v>
+      </c>
+      <c r="E487" s="8" t="s">
+        <v>1098</v>
+      </c>
+      <c r="F487" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G487" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="H487" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="I487" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J487" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="K487" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="L487" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="M487" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="488" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A488" s="4">
+        <v>45613.038227060184</v>
+      </c>
+      <c r="B488" s="5" t="s">
+        <v>1099</v>
+      </c>
+      <c r="C488" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D488" s="5">
+        <v>20217180</v>
+      </c>
+      <c r="E488" s="5" t="s">
+        <v>1100</v>
+      </c>
+      <c r="F488" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G488" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H488" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="I488" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J488" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="K488" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="L488" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="M488" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="489" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A489" s="7">
+        <v>45613.041577175929</v>
+      </c>
+      <c r="B489" s="8" t="s">
+        <v>1101</v>
+      </c>
+      <c r="C489" s="8" t="s">
+        <v>1027</v>
+      </c>
+      <c r="D489" s="8">
+        <v>20192983</v>
+      </c>
+      <c r="E489" s="8" t="s">
+        <v>1102</v>
+      </c>
+      <c r="F489" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G489" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H489" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="I489" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J489" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K489" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="L489" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="M489" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="490" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A490" s="4">
+        <v>45613.041591296293</v>
+      </c>
+      <c r="B490" s="5" t="s">
+        <v>1103</v>
+      </c>
+      <c r="C490" s="5" t="s">
+        <v>583</v>
+      </c>
+      <c r="D490" s="5">
+        <v>20206623</v>
+      </c>
+      <c r="E490" s="5" t="s">
+        <v>1104</v>
+      </c>
+      <c r="F490" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G490" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H490" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I490" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J490" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="K490" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="L490" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N490" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="491" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A491" s="7">
+        <v>45613.045521747685</v>
+      </c>
+      <c r="B491" s="8" t="s">
+        <v>1105</v>
+      </c>
+      <c r="C491" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="D491" s="8">
+        <v>20246610</v>
+      </c>
+      <c r="E491" s="8" t="s">
+        <v>1106</v>
+      </c>
+      <c r="F491" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G491" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="H491" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="I491" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J491" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="K491" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="L491" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="M491" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="492" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A492" s="4">
+        <v>45613.048420370367</v>
+      </c>
+      <c r="B492" s="5" t="s">
+        <v>1107</v>
+      </c>
+      <c r="C492" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="D492" s="5">
+        <v>20243238</v>
+      </c>
+      <c r="E492" s="5" t="s">
+        <v>1108</v>
+      </c>
+      <c r="F492" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="G492" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H492" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="I492" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="J492" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="K492" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="L492" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="M492" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="493" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A493" s="7">
+        <v>45613.067563194447</v>
+      </c>
+      <c r="B493" s="8" t="s">
+        <v>1109</v>
+      </c>
+      <c r="C493" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D493" s="8">
+        <v>20243703</v>
+      </c>
+      <c r="E493" s="8" t="s">
+        <v>1110</v>
+      </c>
+      <c r="F493" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G493" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H493" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="I493" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J493" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="K493" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="L493" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="N493" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="494" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A494" s="4">
+        <v>45613.074090844908</v>
+      </c>
+      <c r="B494" s="5" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C494" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="D494" s="5">
+        <v>20227037</v>
+      </c>
+      <c r="E494" s="5" t="s">
+        <v>1112</v>
+      </c>
+      <c r="F494" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G494" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H494" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="I494" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J494" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="K494" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="L494" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="M494" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="495" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A495" s="7">
+        <v>45613.079241099535</v>
+      </c>
+      <c r="B495" s="8" t="s">
+        <v>1113</v>
+      </c>
+      <c r="C495" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D495" s="8">
+        <v>20242618</v>
+      </c>
+      <c r="E495" s="8" t="s">
+        <v>1114</v>
+      </c>
+      <c r="F495" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G495" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="H495" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="I495" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J495" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="K495" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="L495" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="M495" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="496" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A496" s="4">
+        <v>45613.121412673616</v>
+      </c>
+      <c r="B496" s="5" t="s">
+        <v>1115</v>
+      </c>
+      <c r="C496" s="5" t="s">
+        <v>796</v>
+      </c>
+      <c r="D496" s="5">
+        <v>20191106</v>
+      </c>
+      <c r="E496" s="5" t="s">
+        <v>1116</v>
+      </c>
+      <c r="F496" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G496" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H496" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="I496" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J496" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="K496" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="L496" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N496" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="497" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A497" s="7">
+        <v>45613.138158287038</v>
+      </c>
+      <c r="B497" s="8" t="s">
+        <v>1117</v>
+      </c>
+      <c r="C497" s="8" t="s">
+        <v>277</v>
+      </c>
+      <c r="D497" s="8">
+        <v>20245176</v>
+      </c>
+      <c r="E497" s="8" t="s">
+        <v>1118</v>
+      </c>
+      <c r="F497" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G497" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H497" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="I497" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J497" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K497" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="L497" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="M497" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="498" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A498" s="4">
+        <v>45613.215964016199</v>
+      </c>
+      <c r="B498" s="5" t="s">
+        <v>1119</v>
+      </c>
+      <c r="C498" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D498" s="5">
+        <v>20227143</v>
+      </c>
+      <c r="E498" s="5" t="s">
+        <v>1120</v>
+      </c>
+      <c r="F498" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G498" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H498" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="I498" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J498" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="K498" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="L498" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="M498" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="499" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A499" s="7">
+        <v>45613.273142986116</v>
+      </c>
+      <c r="B499" s="8" t="s">
+        <v>1121</v>
+      </c>
+      <c r="C499" s="8" t="s">
+        <v>1122</v>
+      </c>
+      <c r="D499" s="8">
+        <v>20203322</v>
+      </c>
+      <c r="E499" s="8" t="s">
+        <v>1123</v>
+      </c>
+      <c r="F499" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G499" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H499" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I499" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="J499" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="K499" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="L499" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="M499" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="500" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A500" s="13">
+        <v>45613.311094340279</v>
+      </c>
+      <c r="B500" s="14" t="s">
+        <v>1124</v>
+      </c>
+      <c r="C500" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="D500" s="14">
+        <v>20244123</v>
+      </c>
+      <c r="E500" s="14" t="s">
+        <v>1125</v>
+      </c>
+      <c r="F500" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="G500" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="H500" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="I500" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="J500" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="K500" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="L500" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="M500" s="14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="501" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A501" s="7">
+        <v>45613.335500775458</v>
+      </c>
+      <c r="B501" s="8" t="s">
+        <v>1138</v>
+      </c>
+      <c r="C501" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="D501" s="8">
+        <v>20203616</v>
+      </c>
+      <c r="E501" s="8" t="s">
+        <v>1139</v>
+      </c>
+      <c r="F501" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G501" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H501" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I501" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="J501" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="K501" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="L501" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="N501" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="502" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A502" s="4">
+        <v>45613.335779618057</v>
+      </c>
+      <c r="B502" s="5" t="s">
+        <v>1140</v>
+      </c>
+      <c r="C502" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D502" s="5">
+        <v>20243038</v>
+      </c>
+      <c r="E502" s="5" t="s">
+        <v>1141</v>
+      </c>
+      <c r="F502" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G502" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H502" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I502" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="J502" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="K502" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="L502" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="M502" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="503" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A503" s="7">
+        <v>45613.340120729168</v>
+      </c>
+      <c r="B503" s="8" t="s">
+        <v>1142</v>
+      </c>
+      <c r="C503" s="8" t="s">
+        <v>1143</v>
+      </c>
+      <c r="D503" s="8">
+        <v>20193341</v>
+      </c>
+      <c r="E503" s="8" t="s">
+        <v>1144</v>
+      </c>
+      <c r="F503" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G503" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="H503" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="I503" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="J503" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K503" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="L503" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="N503" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="504" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A504" s="4">
+        <v>45613.342386261575</v>
+      </c>
+      <c r="B504" s="5" t="s">
+        <v>1126</v>
+      </c>
+      <c r="C504" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D504" s="5">
+        <v>20161632</v>
+      </c>
+      <c r="E504" s="5" t="s">
+        <v>1127</v>
+      </c>
+      <c r="F504" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="G504" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H504" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="I504" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J504" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="K504" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="L504" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="M504" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="505" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A505" s="7">
+        <v>45613.351256979164</v>
+      </c>
+      <c r="B505" s="8" t="s">
+        <v>1130</v>
+      </c>
+      <c r="C505" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="D505" s="8">
+        <v>20241510</v>
+      </c>
+      <c r="E505" s="8" t="s">
+        <v>1131</v>
+      </c>
+      <c r="F505" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G505" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="H505" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I505" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J505" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="K505" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="L505" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="N505" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="506" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A506" s="4">
+        <v>45613.35156894676</v>
+      </c>
+      <c r="B506" s="5" t="s">
+        <v>1128</v>
+      </c>
+      <c r="C506" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D506" s="5">
+        <v>20246203</v>
+      </c>
+      <c r="E506" s="5" t="s">
+        <v>1129</v>
+      </c>
+      <c r="F506" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G506" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H506" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I506" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J506" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="K506" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="L506" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="M506" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="507" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A507" s="7">
+        <v>45613.380008611115</v>
+      </c>
+      <c r="B507" s="8" t="s">
+        <v>1132</v>
+      </c>
+      <c r="C507" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="D507" s="8">
+        <v>20221717</v>
+      </c>
+      <c r="E507" s="8" t="s">
+        <v>1133</v>
+      </c>
+      <c r="F507" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G507" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="H507" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="I507" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="J507" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="K507" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="L507" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="M507" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="508" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A508" s="4">
+        <v>45613.427982048612</v>
+      </c>
+      <c r="B508" s="5" t="s">
+        <v>1136</v>
+      </c>
+      <c r="C508" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="D508" s="5">
+        <v>20202324</v>
+      </c>
+      <c r="E508" s="5" t="s">
+        <v>1137</v>
+      </c>
+      <c r="F508" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G508" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H508" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I508" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J508" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="K508" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="L508" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="M508" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="509" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A509" s="17">
+        <v>45613.43532340278</v>
+      </c>
+      <c r="B509" s="18" t="s">
+        <v>1134</v>
+      </c>
+      <c r="C509" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="D509" s="18">
+        <v>20242532</v>
+      </c>
+      <c r="E509" s="18" t="s">
+        <v>1135</v>
+      </c>
+      <c r="F509" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="G509" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="H509" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="I509" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="J509" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="K509" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="L509" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="M509" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="N509" s="20"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>